<commit_message>
Added 1-wire temperature sensor (dirty edit)
Added 1-wire temperature sensor (dirty edit)
</commit_message>
<xml_diff>
--- a/Hardware pinout.xlsx
+++ b/Hardware pinout.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OGRIN\Dropbox\EleksTubeIPS\EleksTubeHAX_AO\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7899FC6B-57DF-4437-A31F-C745219448D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28995" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="All the pins" sheetId="1" r:id="rId1"/>
@@ -20,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="275">
   <si>
     <t>No.</t>
   </si>
@@ -839,12 +833,18 @@
   </si>
   <si>
     <t>DSP 11 TFT - CLOCK</t>
+  </si>
+  <si>
+    <t>nc (via)</t>
+  </si>
+  <si>
+    <t>DS18B20 temp sensor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1032,7 +1032,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Navadno" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1244,38 +1244,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:U56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="S27" sqref="S27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.3984375" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" customWidth="1"/>
+    <col min="3" max="3" width="5.73046875" customWidth="1"/>
+    <col min="4" max="4" width="7.59765625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="10" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" customWidth="1"/>
-    <col min="9" max="9" width="6.85546875" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.73046875" customWidth="1"/>
+    <col min="7" max="7" width="11.3984375" style="10" customWidth="1"/>
+    <col min="8" max="8" width="8.265625" customWidth="1"/>
+    <col min="9" max="9" width="6.86328125" customWidth="1"/>
+    <col min="10" max="10" width="5.59765625" customWidth="1"/>
     <col min="11" max="11" width="6" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.86328125" customWidth="1"/>
     <col min="13" max="13" width="7" customWidth="1"/>
-    <col min="14" max="14" width="13.140625" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" customWidth="1"/>
-    <col min="17" max="17" width="15.28515625" customWidth="1"/>
-    <col min="18" max="18" width="30.28515625" customWidth="1"/>
+    <col min="14" max="14" width="13.1328125" customWidth="1"/>
+    <col min="15" max="15" width="6.73046875" customWidth="1"/>
+    <col min="16" max="16" width="11.265625" customWidth="1"/>
+    <col min="17" max="17" width="15.265625" customWidth="1"/>
+    <col min="18" max="18" width="30.265625" customWidth="1"/>
     <col min="19" max="20" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
@@ -1338,7 +1340,7 @@
       </c>
       <c r="U1" s="12"/>
     </row>
-    <row r="2" spans="1:21" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1371,7 +1373,7 @@
       </c>
       <c r="U2" s="6"/>
     </row>
-    <row r="3" spans="1:21" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1404,7 +1406,7 @@
       </c>
       <c r="U3" s="6"/>
     </row>
-    <row r="4" spans="1:21" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="19">
         <v>3</v>
       </c>
@@ -1437,7 +1439,7 @@
       </c>
       <c r="U4" s="6"/>
     </row>
-    <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1480,7 +1482,7 @@
       </c>
       <c r="U5" s="1"/>
     </row>
-    <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1523,7 +1525,7 @@
       </c>
       <c r="U6" s="2"/>
     </row>
-    <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1566,7 +1568,7 @@
       </c>
       <c r="U7" s="2"/>
     </row>
-    <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1609,7 +1611,7 @@
       </c>
       <c r="U8" s="2"/>
     </row>
-    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1651,7 +1653,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1694,7 +1696,7 @@
       </c>
       <c r="U10" s="2"/>
     </row>
-    <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1737,7 +1739,7 @@
       </c>
       <c r="U11" s="2"/>
     </row>
-    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1780,7 +1782,7 @@
       </c>
       <c r="U12" s="2"/>
     </row>
-    <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1823,7 +1825,7 @@
       </c>
       <c r="U13" s="2"/>
     </row>
-    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1872,7 +1874,7 @@
       </c>
       <c r="U14" s="2"/>
     </row>
-    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="23">
         <v>14</v>
       </c>
@@ -1925,7 +1927,7 @@
       </c>
       <c r="U15" s="2"/>
     </row>
-    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A16" s="32">
         <v>15</v>
       </c>
@@ -1958,7 +1960,7 @@
       </c>
       <c r="U16" s="3"/>
     </row>
-    <row r="17" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="32">
         <v>16</v>
       </c>
@@ -2007,7 +2009,7 @@
       </c>
       <c r="U17" s="2"/>
     </row>
-    <row r="18" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="14">
         <v>17</v>
       </c>
@@ -2054,7 +2056,7 @@
       </c>
       <c r="U18" s="2"/>
     </row>
-    <row r="19" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="14">
         <v>18</v>
       </c>
@@ -2101,7 +2103,7 @@
       </c>
       <c r="U19" s="2"/>
     </row>
-    <row r="20" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="14">
         <v>19</v>
       </c>
@@ -2146,7 +2148,7 @@
       </c>
       <c r="U20" s="2"/>
     </row>
-    <row r="21" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="14">
         <v>20</v>
       </c>
@@ -2193,7 +2195,7 @@
       </c>
       <c r="U21" s="2"/>
     </row>
-    <row r="22" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="14">
         <v>21</v>
       </c>
@@ -2240,7 +2242,7 @@
       </c>
       <c r="U22" s="2"/>
     </row>
-    <row r="23" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="14">
         <v>22</v>
       </c>
@@ -2287,7 +2289,7 @@
       </c>
       <c r="U23" s="2"/>
     </row>
-    <row r="24" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="17">
         <v>23</v>
       </c>
@@ -2338,7 +2340,7 @@
       </c>
       <c r="U24" s="2"/>
     </row>
-    <row r="25" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="23">
         <v>24</v>
       </c>
@@ -2387,7 +2389,7 @@
       </c>
       <c r="U25" s="2"/>
     </row>
-    <row r="26" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="17">
         <v>25</v>
       </c>
@@ -2434,7 +2436,7 @@
       </c>
       <c r="U26" s="2"/>
     </row>
-    <row r="27" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -2473,15 +2475,15 @@
         <v>46</v>
       </c>
       <c r="R27" s="3"/>
-      <c r="S27" s="6" t="s">
-        <v>236</v>
+      <c r="S27" s="42" t="s">
+        <v>274</v>
       </c>
       <c r="T27" s="3" t="s">
         <v>116</v>
       </c>
       <c r="U27" s="2"/>
     </row>
-    <row r="28" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -2522,7 +2524,7 @@
       </c>
       <c r="U28" s="2"/>
     </row>
-    <row r="29" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -2563,7 +2565,7 @@
       </c>
       <c r="U29" s="2"/>
     </row>
-    <row r="30" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -2606,7 +2608,7 @@
       </c>
       <c r="U30" s="2"/>
     </row>
-    <row r="31" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -2647,7 +2649,7 @@
       </c>
       <c r="U31" s="2"/>
     </row>
-    <row r="32" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -2690,7 +2692,7 @@
       </c>
       <c r="U32" s="2"/>
     </row>
-    <row r="33" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -2713,15 +2715,15 @@
       <c r="P33" s="3"/>
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
-      <c r="S33" s="6" t="s">
-        <v>236</v>
+      <c r="S33" s="42" t="s">
+        <v>273</v>
       </c>
       <c r="T33" s="6" t="s">
         <v>263</v>
       </c>
       <c r="U33" s="3"/>
     </row>
-    <row r="34" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -2762,7 +2764,7 @@
       </c>
       <c r="U34" s="2"/>
     </row>
-    <row r="35" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="17">
         <v>34</v>
       </c>
@@ -2801,7 +2803,7 @@
       <c r="T35" s="22"/>
       <c r="U35" s="2"/>
     </row>
-    <row r="36" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="17">
         <v>35</v>
       </c>
@@ -2842,7 +2844,7 @@
       <c r="T36" s="22"/>
       <c r="U36" s="2"/>
     </row>
-    <row r="37" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -2885,7 +2887,7 @@
       </c>
       <c r="U37" s="2"/>
     </row>
-    <row r="38" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -2926,7 +2928,7 @@
       </c>
       <c r="U38" s="2"/>
     </row>
-    <row r="39" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A39" s="30">
         <v>38</v>
       </c>
@@ -2959,7 +2961,7 @@
       </c>
       <c r="U39" s="2"/>
     </row>
-    <row r="40" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -2982,7 +2984,7 @@
       <c r="T40" s="3"/>
       <c r="U40" s="2"/>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -3011,7 +3013,7 @@
       </c>
       <c r="U41" s="2"/>
     </row>
-    <row r="42" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -3040,7 +3042,7 @@
       </c>
       <c r="U42" s="2"/>
     </row>
-    <row r="43" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -3069,7 +3071,7 @@
       </c>
       <c r="U43" s="2"/>
     </row>
-    <row r="44" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -3098,7 +3100,7 @@
       </c>
       <c r="U44" s="2"/>
     </row>
-    <row r="45" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="R45" s="40">
         <v>4</v>
       </c>
@@ -3109,7 +3111,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="R46" s="40">
         <v>5</v>
       </c>
@@ -3120,7 +3122,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="R47" s="40">
         <v>6</v>
       </c>
@@ -3131,7 +3133,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="R48" s="40">
         <v>7</v>
       </c>
@@ -3142,7 +3144,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="49" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="R49" s="40">
         <v>8</v>
       </c>
@@ -3153,7 +3155,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="50" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="R50" s="40">
         <v>9</v>
       </c>
@@ -3164,7 +3166,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="51" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="R51" s="40">
         <v>10</v>
       </c>
@@ -3175,7 +3177,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="52" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="R52" s="40">
         <v>11</v>
       </c>
@@ -3186,7 +3188,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="53" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="R53" s="40">
         <v>12</v>
       </c>
@@ -3197,7 +3199,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="54" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="R54" s="40">
         <v>13</v>
       </c>
@@ -3208,15 +3210,15 @@
         <v>256</v>
       </c>
     </row>
-    <row r="55" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="S55" s="6"/>
       <c r="T55" s="6"/>
     </row>
-    <row r="56" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="S56" s="6"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:S38">
+  <sortState ref="A5:S38">
     <sortCondition ref="A6:A38"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>